<commit_message>
soubor se 30 lidmi z MIT
</commit_message>
<xml_diff>
--- a/data/kiv/data.xlsx
+++ b/data/kiv/data.xlsx
@@ -1196,9 +1196,6 @@
     <t>Přemysl Brada, Jaroslav Bauml</t>
   </si>
   <si>
-    <t>Přemysl Brada, Kaiml Jažek, Petr Štěpán</t>
-  </si>
-  <si>
     <t>University of West Bohemia, Department of Computer Science and Engineering, Univerzitní 22, 30614, Plzeň, Czech Republic; School of Computer Science, The University of Manchester Manchester M139PL, United Kingdom</t>
   </si>
   <si>
@@ -1302,6 +1299,9 @@
   </si>
   <si>
     <t>Premek Brada, Sangita De, Juergen Mottok, Michael Niklas</t>
+  </si>
+  <si>
+    <t>Přemysl Brada, Kamil Ježek, Petr Štěpán</t>
   </si>
 </sst>
 </file>
@@ -2314,11 +2314,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="166524800"/>
-        <c:axId val="166523264"/>
+        <c:axId val="202028544"/>
+        <c:axId val="202030080"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="166524800"/>
+        <c:axId val="202028544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2328,12 +2328,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166523264"/>
+        <c:crossAx val="202030080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="166523264"/>
+        <c:axId val="202030080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2344,7 +2344,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166524800"/>
+        <c:crossAx val="202028544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2370,16 +2370,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>640080</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>5516880</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>8313420</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2695,7 +2695,7 @@
   <dimension ref="A1:F359"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A301" sqref="A301"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3053,7 +3053,7 @@
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>387</v>
+        <v>422</v>
       </c>
       <c r="C18">
         <v>20</v>
@@ -3065,7 +3065,7 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -3113,7 +3113,7 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C21">
         <v>10</v>
@@ -3133,7 +3133,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C22">
         <v>8</v>
@@ -3153,7 +3153,7 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C23">
         <v>7</v>
@@ -3173,7 +3173,7 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C24">
         <v>5</v>
@@ -3193,7 +3193,7 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -3213,7 +3213,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -3233,7 +3233,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C27">
         <v>11</v>
@@ -3253,7 +3253,7 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -3273,7 +3273,7 @@
         <v>33</v>
       </c>
       <c r="B29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C29">
         <v>5</v>
@@ -3293,7 +3293,7 @@
         <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -3313,7 +3313,7 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -3333,7 +3333,7 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -3353,7 +3353,7 @@
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C33">
         <v>6</v>
@@ -3373,7 +3373,7 @@
         <v>38</v>
       </c>
       <c r="B34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C34">
         <v>3</v>
@@ -3393,7 +3393,7 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C35">
         <v>5</v>
@@ -3413,7 +3413,7 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C36">
         <v>14</v>
@@ -3433,7 +3433,7 @@
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C37">
         <v>8</v>
@@ -3453,7 +3453,7 @@
         <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C38">
         <v>5</v>
@@ -3473,7 +3473,7 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -3493,7 +3493,7 @@
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C40">
         <v>77</v>
@@ -3505,7 +3505,7 @@
         <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -3513,7 +3513,7 @@
         <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C41">
         <v>61</v>
@@ -3525,7 +3525,7 @@
         <v>2</v>
       </c>
       <c r="F41" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -3533,7 +3533,7 @@
         <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C42">
         <v>9</v>
@@ -3553,7 +3553,7 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C43">
         <v>13</v>
@@ -3565,7 +3565,7 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
@@ -3573,7 +3573,7 @@
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C44">
         <v>17</v>
@@ -3585,7 +3585,7 @@
         <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
@@ -3593,7 +3593,7 @@
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -3613,7 +3613,7 @@
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C46">
         <v>14</v>
@@ -3633,7 +3633,7 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -3653,7 +3653,7 @@
         <v>52</v>
       </c>
       <c r="B48" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C48">
         <v>12</v>
@@ -3665,7 +3665,7 @@
         <v>3</v>
       </c>
       <c r="F48" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -3673,7 +3673,7 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C49">
         <v>5</v>
@@ -3693,7 +3693,7 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -3705,7 +3705,7 @@
         <v>2</v>
       </c>
       <c r="F50" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -3713,7 +3713,7 @@
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -3725,7 +3725,7 @@
         <v>3</v>
       </c>
       <c r="F51" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -3733,7 +3733,7 @@
         <v>56</v>
       </c>
       <c r="B52" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C52">
         <v>9</v>
@@ -3753,7 +3753,7 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C53">
         <v>4</v>
@@ -3773,7 +3773,7 @@
         <v>58</v>
       </c>
       <c r="B54" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -3793,7 +3793,7 @@
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -3805,7 +3805,7 @@
         <v>4</v>
       </c>
       <c r="F55" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
@@ -3813,7 +3813,7 @@
         <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -3833,7 +3833,7 @@
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -3853,7 +3853,7 @@
         <v>62</v>
       </c>
       <c r="B58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3865,7 +3865,7 @@
         <v>3</v>
       </c>
       <c r="F58" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -3873,7 +3873,7 @@
         <v>63</v>
       </c>
       <c r="B59" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -3893,7 +3893,7 @@
         <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -3913,7 +3913,7 @@
         <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -3925,7 +3925,7 @@
         <v>4</v>
       </c>
       <c r="F61" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>